<commit_message>
feat(document): add blacklist implementation
</commit_message>
<xml_diff>
--- a/templates/table.xlsx
+++ b/templates/table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\Stockwise\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Stockwise\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF58FCE-47D1-4C9D-A4DF-D86578D1DCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7480D9-DA3B-43A2-97D3-16BEDE6317A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -459,29 +459,28 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.36328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="5" customWidth="1"/>
-    <col min="4" max="6" width="8.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="52.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
+    <col min="4" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="J1" s="2"/>

</xml_diff>